<commit_message>
added sendTo on 4 schemas
</commit_message>
<xml_diff>
--- a/pathfiles/output/JEDxSampleDataSheets2.xlsx
+++ b/pathfiles/output/JEDxSampleDataSheets2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinceparedes/Documents/0_JEDx/P2repo/JEDx/pathfiles/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005F9D6A-846E-B345-AB36-697C0315994A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A950677F-57F3-3840-AFE1-0404305C15C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1380" windowWidth="31740" windowHeight="18400" xr2:uid="{96219773-B60F-5D4E-A95A-7648A8080CF3}"/>
+    <workbookView xWindow="3060" yWindow="1380" windowWidth="31740" windowHeight="18400" activeTab="3" xr2:uid="{96219773-B60F-5D4E-A95A-7648A8080CF3}"/>
   </bookViews>
   <sheets>
     <sheet name="organization" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="274">
   <si>
     <t>Name</t>
   </si>
@@ -842,6 +842,18 @@
   </si>
   <si>
     <t>organization.tradeName</t>
+  </si>
+  <si>
+    <t>same as organization state</t>
+  </si>
+  <si>
+    <t>BasePay</t>
+  </si>
+  <si>
+    <t>OtherPremium</t>
+  </si>
+  <si>
+    <t>Holiday</t>
   </si>
 </sst>
 </file>
@@ -1778,7 +1790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B6A5D4-7AC2-EE44-982B-E711F9F70332}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="130" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="130" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -2609,8 +2621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33006760-66C3-5549-A3CF-3FA229F4EC24}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScale="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="C1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2869,7 +2881,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>153</v>
       </c>
@@ -2883,7 +2895,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>156</v>
       </c>
@@ -2897,7 +2909,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>159</v>
       </c>
@@ -2911,7 +2923,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -2925,7 +2937,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -2939,7 +2951,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -2953,7 +2965,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -2966,8 +2978,11 @@
       <c r="D23" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2980,8 +2995,11 @@
       <c r="D24" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -2992,7 +3010,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -3003,7 +3021,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -3014,7 +3032,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -3028,7 +3046,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -3042,7 +3060,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -3056,7 +3074,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>96</v>
       </c>
@@ -3070,7 +3088,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -3120,8 +3138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0751570-123D-B74E-B22D-CEA898BBE8FD}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3129,8 +3147,8 @@
     <col min="1" max="1" width="34" style="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="1" customWidth="1"/>
     <col min="3" max="3" width="34" style="1" customWidth="1"/>
-    <col min="4" max="4" width="74.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="83.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.83203125" style="1" customWidth="1"/>
     <col min="7" max="8" width="34" style="1" customWidth="1"/>
   </cols>
@@ -3413,6 +3431,9 @@
       <c r="D18" s="1" t="s">
         <v>207</v>
       </c>
+      <c r="E18" s="1" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -3466,6 +3487,9 @@
       <c r="D22" s="1" t="s">
         <v>214</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -3519,6 +3543,9 @@
       <c r="D26" s="1" t="s">
         <v>220</v>
       </c>
+      <c r="E26" s="1" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
@@ -3557,6 +3584,9 @@
       </c>
       <c r="D29" s="1" t="s">
         <v>224</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>